<commit_message>
Add XLSX reading example
</commit_message>
<xml_diff>
--- a/spreadsheets/xls_example.xlsx
+++ b/spreadsheets/xls_example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t xml:space="preserve">TABLE:  Joint Reactions</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t xml:space="preserve">MAX-N BEAM CARAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11300030</t>
   </si>
   <si>
     <t xml:space="preserve">MIN-N BEAM CARAC</t>
@@ -146,8 +143,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -213,8 +211,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -238,10 +240,13 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F4:K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.44"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -313,8 +318,8 @@
       <c r="B4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>16</v>
+      <c r="C4" s="0" t="n">
+        <v>11300030</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0.524</v>
@@ -322,22 +327,22 @@
       <c r="E4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>-7731</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>1194</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="1" t="n">
         <v>-594</v>
       </c>
-      <c r="I4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="0" t="n">
+      <c r="I4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1" t="n">
         <v>-4671</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="1" t="n">
         <v>-9384</v>
       </c>
     </row>
@@ -346,7 +351,7 @@
         <v>34022</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>11300030</v>
@@ -357,22 +362,22 @@
       <c r="E5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>-15243</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>-311</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>306</v>
       </c>
-      <c r="I5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="0" t="n">
+      <c r="I5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1" t="n">
         <v>2409</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="K5" s="1" t="n">
         <v>2442</v>
       </c>
     </row>
@@ -381,7 +386,7 @@
         <v>34023</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>11300030</v>
@@ -392,22 +397,22 @@
       <c r="E6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>-8239</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>1767</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="1" t="n">
         <v>-368</v>
       </c>
-      <c r="I6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="0" t="n">
+      <c r="I6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1" t="n">
         <v>-2894</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6" s="1" t="n">
         <v>-13890</v>
       </c>
     </row>
@@ -416,7 +421,7 @@
         <v>34024</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>11300030</v>
@@ -427,22 +432,22 @@
       <c r="E7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>-14742</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>-882</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="I7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="0" t="n">
+      <c r="I7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1" t="n">
         <v>1842.75</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="K7" s="1" t="n">
         <v>6936</v>
       </c>
     </row>
@@ -451,7 +456,7 @@
         <v>34025</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>11300030</v>
@@ -462,22 +467,22 @@
       <c r="E8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>-14740</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>-755</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="1" t="n">
         <v>452</v>
       </c>
-      <c r="I8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="0" t="n">
+      <c r="I8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1" t="n">
         <v>3554</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="K8" s="1" t="n">
         <v>5938</v>
       </c>
     </row>
@@ -486,7 +491,7 @@
         <v>34026</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>11300030</v>
@@ -497,22 +502,22 @@
       <c r="E9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>-8241</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>1640</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="1" t="n">
         <v>-740</v>
       </c>
-      <c r="I9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="0" t="n">
+      <c r="I9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1" t="n">
         <v>-5819</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="K9" s="1" t="n">
         <v>-12892</v>
       </c>
     </row>
@@ -521,7 +526,7 @@
         <v>34027</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>11300030</v>
@@ -532,22 +537,22 @@
       <c r="E10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>-7731</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>1194</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="1" t="n">
         <v>-594</v>
       </c>
-      <c r="I10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="0" t="n">
+      <c r="I10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1" t="n">
         <v>-4671</v>
       </c>
-      <c r="K10" s="0" t="n">
+      <c r="K10" s="1" t="n">
         <v>-9384</v>
       </c>
     </row>
@@ -556,7 +561,7 @@
         <v>34028</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>11300030</v>
@@ -567,22 +572,22 @@
       <c r="E11" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <v>-7731</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>1194</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="1" t="n">
         <v>-594</v>
       </c>
-      <c r="I11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" s="0" t="n">
+      <c r="I11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1" t="n">
         <v>-4671</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="K11" s="1" t="n">
         <v>-9384</v>
       </c>
     </row>
@@ -591,7 +596,7 @@
         <v>34029</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>11300030</v>
@@ -602,22 +607,22 @@
       <c r="E12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="1" t="n">
         <v>-14740</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="1" t="n">
         <v>-755</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12" s="1" t="n">
         <v>452</v>
       </c>
-      <c r="I12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="0" t="n">
+      <c r="I12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1" t="n">
         <v>3554</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="K12" s="1" t="n">
         <v>5938</v>
       </c>
     </row>
@@ -626,7 +631,7 @@
         <v>34030</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>11300030</v>
@@ -637,22 +642,22 @@
       <c r="E13" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <v>-8241</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="1" t="n">
         <v>1640</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13" s="1" t="n">
         <v>-740</v>
       </c>
-      <c r="I13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="0" t="n">
+      <c r="I13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1" t="n">
         <v>-5819</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="K13" s="1" t="n">
         <v>-12892</v>
       </c>
     </row>
@@ -661,7 +666,7 @@
         <v>34031</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>11300030</v>
@@ -672,22 +677,22 @@
       <c r="E14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="1" t="n">
         <v>-14742</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="1" t="n">
         <v>-882</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="I14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="0" t="n">
+      <c r="I14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1" t="n">
         <v>1842.75</v>
       </c>
-      <c r="K14" s="0" t="n">
+      <c r="K14" s="1" t="n">
         <v>6936</v>
       </c>
     </row>
@@ -696,7 +701,7 @@
         <v>34032</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>11300030</v>
@@ -707,22 +712,22 @@
       <c r="E15" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="1" t="n">
         <v>-8239</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="1" t="n">
         <v>1767</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15" s="1" t="n">
         <v>-368</v>
       </c>
-      <c r="I15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" s="0" t="n">
+      <c r="I15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1" t="n">
         <v>-2894</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="K15" s="1" t="n">
         <v>-13890</v>
       </c>
     </row>
@@ -731,7 +736,7 @@
         <v>14021</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>11300030</v>
@@ -742,22 +747,22 @@
       <c r="E16" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <v>-7096</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="1" t="n">
         <v>1694</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16" s="1" t="n">
         <v>-829</v>
       </c>
-      <c r="I16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" s="0" t="n">
+      <c r="I16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1" t="n">
         <v>-6514</v>
       </c>
-      <c r="K16" s="0" t="n">
+      <c r="K16" s="1" t="n">
         <v>-13313</v>
       </c>
     </row>
@@ -766,7 +771,7 @@
         <v>14022</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>11300030</v>
@@ -777,22 +782,22 @@
       <c r="E17" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="1" t="n">
         <v>-21284</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="1" t="n">
         <v>-925</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="H17" s="1" t="n">
         <v>578</v>
       </c>
-      <c r="I17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" s="0" t="n">
+      <c r="I17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1" t="n">
         <v>4542</v>
       </c>
-      <c r="K17" s="0" t="n">
+      <c r="K17" s="1" t="n">
         <v>7267</v>
       </c>
     </row>
@@ -801,7 +806,7 @@
         <v>14023</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>11300030</v>
@@ -812,22 +817,22 @@
       <c r="E18" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="1" t="n">
         <v>-7908</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="1" t="n">
         <v>2368</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H18" s="1" t="n">
         <v>-491</v>
       </c>
-      <c r="I18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" s="0" t="n">
+      <c r="I18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1" t="n">
         <v>-3860</v>
       </c>
-      <c r="K18" s="0" t="n">
+      <c r="K18" s="1" t="n">
         <v>-18610</v>
       </c>
     </row>
@@ -836,7 +841,7 @@
         <v>14024</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>11300030</v>
@@ -847,22 +852,22 @@
       <c r="E19" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="1" t="n">
         <v>-20483</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="1" t="n">
         <v>-1596</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="H19" s="1" t="n">
         <v>239</v>
       </c>
-      <c r="I19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" s="0" t="n">
+      <c r="I19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1" t="n">
         <v>1882</v>
       </c>
-      <c r="K19" s="0" t="n">
+      <c r="K19" s="1" t="n">
         <v>12546</v>
       </c>
     </row>
@@ -871,7 +876,7 @@
         <v>14025</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>11300030</v>
@@ -882,22 +887,22 @@
       <c r="E20" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="1" t="n">
         <v>-20480</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="G20" s="1" t="n">
         <v>-1425</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="H20" s="1" t="n">
         <v>742</v>
       </c>
-      <c r="I20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" s="0" t="n">
+      <c r="I20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1" t="n">
         <v>5832</v>
       </c>
-      <c r="K20" s="0" t="n">
+      <c r="K20" s="1" t="n">
         <v>11199</v>
       </c>
     </row>
@@ -906,7 +911,7 @@
         <v>14026</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>11300030</v>
@@ -917,22 +922,22 @@
       <c r="E21" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="1" t="n">
         <v>-7912</v>
       </c>
-      <c r="G21" s="0" t="n">
+      <c r="G21" s="1" t="n">
         <v>2196</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="H21" s="1" t="n">
         <v>-994</v>
       </c>
-      <c r="I21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="0" t="n">
+      <c r="I21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1" t="n">
         <v>-7810</v>
       </c>
-      <c r="K21" s="0" t="n">
+      <c r="K21" s="1" t="n">
         <v>-17262</v>
       </c>
     </row>
@@ -941,7 +946,7 @@
         <v>14027</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>11300030</v>
@@ -952,22 +957,22 @@
       <c r="E22" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22" s="1" t="n">
         <v>-7096</v>
       </c>
-      <c r="G22" s="0" t="n">
+      <c r="G22" s="1" t="n">
         <v>1694</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="H22" s="1" t="n">
         <v>-829</v>
       </c>
-      <c r="I22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" s="0" t="n">
+      <c r="I22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1" t="n">
         <v>-6514</v>
       </c>
-      <c r="K22" s="0" t="n">
+      <c r="K22" s="1" t="n">
         <v>-13313</v>
       </c>
     </row>
@@ -976,7 +981,7 @@
         <v>14028</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>11300030</v>
@@ -987,22 +992,22 @@
       <c r="E23" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="F23" s="1" t="n">
         <v>-7096</v>
       </c>
-      <c r="G23" s="0" t="n">
+      <c r="G23" s="1" t="n">
         <v>1694</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="H23" s="1" t="n">
         <v>-829</v>
       </c>
-      <c r="I23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" s="0" t="n">
+      <c r="I23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1" t="n">
         <v>-6514</v>
       </c>
-      <c r="K23" s="0" t="n">
+      <c r="K23" s="1" t="n">
         <v>-13313</v>
       </c>
     </row>
@@ -1011,7 +1016,7 @@
         <v>14029</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>11300030</v>
@@ -1022,22 +1027,22 @@
       <c r="E24" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="F24" s="1" t="n">
         <v>-20480</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="G24" s="1" t="n">
         <v>-1425</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="H24" s="1" t="n">
         <v>742</v>
       </c>
-      <c r="I24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J24" s="0" t="n">
+      <c r="I24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1" t="n">
         <v>5832</v>
       </c>
-      <c r="K24" s="0" t="n">
+      <c r="K24" s="1" t="n">
         <v>11199</v>
       </c>
     </row>
@@ -1046,7 +1051,7 @@
         <v>14030</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>11300030</v>
@@ -1057,22 +1062,22 @@
       <c r="E25" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25" s="1" t="n">
         <v>-7912</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="G25" s="1" t="n">
         <v>2196</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="H25" s="1" t="n">
         <v>-994</v>
       </c>
-      <c r="I25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J25" s="0" t="n">
+      <c r="I25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="1" t="n">
         <v>-7810</v>
       </c>
-      <c r="K25" s="0" t="n">
+      <c r="K25" s="1" t="n">
         <v>-17262</v>
       </c>
     </row>
@@ -1081,7 +1086,7 @@
         <v>14031</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>11300030</v>
@@ -1092,22 +1097,22 @@
       <c r="E26" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26" s="1" t="n">
         <v>-20483</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="G26" s="1" t="n">
         <v>-1596</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="H26" s="1" t="n">
         <v>239</v>
       </c>
-      <c r="I26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J26" s="0" t="n">
+      <c r="I26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1" t="n">
         <v>1882</v>
       </c>
-      <c r="K26" s="0" t="n">
+      <c r="K26" s="1" t="n">
         <v>12546</v>
       </c>
     </row>
@@ -1116,7 +1121,7 @@
         <v>14032</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>11300030</v>
@@ -1127,22 +1132,22 @@
       <c r="E27" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27" s="1" t="n">
         <v>-7908</v>
       </c>
-      <c r="G27" s="0" t="n">
+      <c r="G27" s="1" t="n">
         <v>2368</v>
       </c>
-      <c r="H27" s="0" t="n">
+      <c r="H27" s="1" t="n">
         <v>-491</v>
       </c>
-      <c r="I27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" s="0" t="n">
+      <c r="I27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="1" t="n">
         <v>-3860</v>
       </c>
-      <c r="K27" s="0" t="n">
+      <c r="K27" s="1" t="n">
         <v>-18610</v>
       </c>
     </row>

</xml_diff>